<commit_message>
Update example template with VERSION sheet
</commit_message>
<xml_diff>
--- a/examples/LLC_Accounting_Template.xlsx
+++ b/examples/LLC_Accounting_Template.xlsx
@@ -9,13 +9,14 @@
     <sheet sheetId="3" name="Credit Card Transactions" state="visible" r:id="rId6"/>
     <sheet sheetId="4" name="Ledger" state="visible" r:id="rId7"/>
     <sheet sheetId="5" name="Summary" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="VERSION" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Category</t>
   </si>
@@ -62,6 +63,9 @@
     <t>P&amp;L</t>
   </si>
   <si>
+    <t>Starbucks</t>
+  </si>
+  <si>
     <t>Bank Transactions</t>
   </si>
   <si>
@@ -80,6 +84,9 @@
     <t>Expense</t>
   </si>
   <si>
+    <t>Amazon</t>
+  </si>
+  <si>
     <t>Credit Card Transactions</t>
   </si>
   <si>
@@ -98,6 +105,9 @@
     <t>Balance Sheet</t>
   </si>
   <si>
+    <t>AWS</t>
+  </si>
+  <si>
     <t>Credit Card</t>
   </si>
   <si>
@@ -141,6 +151,30 @@
   </si>
   <si>
     <t>Credit</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Version ID</t>
+  </si>
+  <si>
+    <t>1.0.0-java</t>
+  </si>
+  <si>
+    <t>Git SHA</t>
+  </si>
+  <si>
+    <t>fa8999fc0a5c37c5e114a44cb01475b5da278394</t>
+  </si>
+  <si>
+    <t>Generated At</t>
+  </si>
+  <si>
+    <t>12/22/2025, 10:07:03 AM</t>
   </si>
 </sst>
 </file>
@@ -582,14 +616,17 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -597,70 +634,76 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -685,13 +728,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -700,16 +743,16 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -738,16 +781,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -756,22 +799,22 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
         <v>39</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -794,22 +837,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -826,4 +869,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>